<commit_message>
add, trans FAQ page
</commit_message>
<xml_diff>
--- a/chatbot/Don_vi_Can_Tho.xlsx
+++ b/chatbot/Don_vi_Can_Tho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deadline\LV\PolygonApplication\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CAFA1-FB04-4957-95EC-EC14E5110985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD3846C-F12F-45FA-B597-4CBC16B6FBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1824,7 +1824,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>